<commit_message>
Reverted some attribute names in MEDICATION, BILL, PAYMENT. Also added group enum for patient and schedule
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -145,6 +145,12 @@
     <t xml:space="preserve">admission_date</t>
   </si>
   <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enum (‘red’, ‘blue’, ‘green’, ‘yellow)</t>
+  </si>
+  <si>
     <t xml:space="preserve">int FK (USER)</t>
   </si>
   <si>
@@ -160,6 +166,9 @@
     <t xml:space="preserve">hire_date</t>
   </si>
   <si>
+    <t xml:space="preserve">appt_date</t>
+  </si>
+  <si>
     <t xml:space="preserve">salary</t>
   </si>
   <si>
@@ -184,16 +193,19 @@
     <t xml:space="preserve">med_id</t>
   </si>
   <si>
-    <t xml:space="preserve">amount</t>
+    <t xml:space="preserve">bill_amount</t>
   </si>
   <si>
     <t xml:space="preserve">int NOT NULL</t>
   </si>
   <si>
+    <t xml:space="preserve">med_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">creation_date</t>
   </si>
   <si>
-    <t xml:space="preserve">dose</t>
+    <t xml:space="preserve">med_dose</t>
   </si>
   <si>
     <t xml:space="preserve">Varchar(25) NOT NULL</t>
@@ -202,7 +214,7 @@
     <t xml:space="preserve">due_date </t>
   </si>
   <si>
-    <t xml:space="preserve">quantity</t>
+    <t xml:space="preserve">med_quantity</t>
   </si>
   <si>
     <t xml:space="preserve">INT FK (PATIENT)</t>
@@ -220,6 +232,9 @@
     <t xml:space="preserve">payment_id</t>
   </si>
   <si>
+    <t xml:space="preserve">payment_amount</t>
+  </si>
+  <si>
     <t xml:space="preserve">made_by</t>
   </si>
   <si>
@@ -235,7 +250,7 @@
     <t xml:space="preserve">care_red</t>
   </si>
   <si>
-    <t xml:space="preserve">int FK (GROUP) NOT NULL</t>
+    <t xml:space="preserve">enum (‘red’, ‘blue’, ‘green’, ‘yellow) FK PATIENT</t>
   </si>
   <si>
     <t xml:space="preserve">care_blue</t>
@@ -358,10 +373,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,7 +435,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -480,7 +495,7 @@
       <c r="B9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="0" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="0" t="s">
@@ -507,7 +522,6 @@
       <c r="E11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -591,19 +605,27 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>41</v>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -615,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>3</v>
@@ -623,13 +645,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>14</v>
@@ -637,7 +659,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>8</v>
@@ -646,42 +668,42 @@
         <v>27</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>41</v>
+      <c r="B25" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>3</v>
@@ -689,13 +711,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>6</v>
@@ -703,27 +725,27 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>8</v>
@@ -740,36 +762,36 @@
         <v>27</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>3</v>
@@ -783,21 +805,21 @@
         <v>14</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>14</v>
@@ -805,56 +827,56 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>71</v>
+      <c r="A42" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>71</v>
+      <c r="A43" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>71</v>
+      <c r="A44" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -871,11 +893,11 @@
     <mergeCell ref="D35:E35"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced USER 'name' with 'fname' and 'lname'
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">role_id</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
+    <t xml:space="preserve">fname</t>
   </si>
   <si>
     <t xml:space="preserve">Varchar(50) NOT NULL</t>
@@ -55,10 +55,13 @@
     <t xml:space="preserve">Varchar(255) NOT NULL</t>
   </si>
   <si>
+    <t xml:space="preserve">CARE</t>
+  </si>
+  <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">CARE</t>
+    <t xml:space="preserve">record_id</t>
   </si>
   <si>
     <t xml:space="preserve">dob</t>
@@ -67,7 +70,10 @@
     <t xml:space="preserve">date NOT NULL</t>
   </si>
   <si>
-    <t xml:space="preserve">record_id</t>
+    <t xml:space="preserve">med_morn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool</t>
   </si>
   <si>
     <t xml:space="preserve">phone</t>
@@ -76,22 +82,16 @@
     <t xml:space="preserve">Varchar(10)</t>
   </si>
   <si>
-    <t xml:space="preserve">med_morn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bool</t>
+    <t xml:space="preserve">med_noon</t>
   </si>
   <si>
     <t xml:space="preserve">approved</t>
   </si>
   <si>
-    <t xml:space="preserve">med_noon</t>
+    <t xml:space="preserve">med_night</t>
   </si>
   <si>
     <t xml:space="preserve">Varchar(20) FK (ACCESS_ROLES)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_night</t>
   </si>
   <si>
     <t xml:space="preserve">breakfast</t>
@@ -339,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,10 +350,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -376,7 +372,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,33 +424,33 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>3</v>
@@ -462,53 +458,58 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3"/>
       <c r="D10" s="0" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +521,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,7 +535,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,7 +585,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,7 +601,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,13 +649,13 @@
         <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,7 +729,7 @@
         <v>60</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>61</v>
@@ -742,7 +743,7 @@
         <v>63</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>64</v>
@@ -802,7 +803,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>70</v>
@@ -822,7 +823,7 @@
         <v>72</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed USER having two 'fnames' (one is now 'lname')
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lname</t>
   </si>
   <si>
     <t xml:space="preserve">email</t>
@@ -372,7 +375,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,7 +427,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
@@ -432,25 +435,25 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>3</v>
@@ -458,44 +461,44 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,113 +506,113 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2"/>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,28 +620,28 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>3</v>
@@ -646,30 +649,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,34 +680,34 @@
         <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>3</v>
@@ -712,13 +715,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>6</v>
@@ -726,27 +729,27 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>8</v>
@@ -754,45 +757,45 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>3</v>
@@ -800,84 +803,84 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed PATIENT group and the groups in SCHEDULE
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -43,15 +43,21 @@
     <t xml:space="preserve">Varchar(50) NOT NULL</t>
   </si>
   <si>
+    <t xml:space="preserve">role_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar(20) NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lname</t>
+  </si>
+  <si>
     <t xml:space="preserve">access_level</t>
   </si>
   <si>
     <t xml:space="preserve">int </t>
   </si>
   <si>
-    <t xml:space="preserve">lname</t>
-  </si>
-  <si>
     <t xml:space="preserve">email</t>
   </si>
   <si>
@@ -94,7 +100,7 @@
     <t xml:space="preserve">med_night</t>
   </si>
   <si>
-    <t xml:space="preserve">Varchar(20) FK (ACCESS_ROLES)</t>
+    <t xml:space="preserve">role_id FK (ACCESS_ROLES)</t>
   </si>
   <si>
     <t xml:space="preserve">breakfast</t>
@@ -251,9 +257,6 @@
   </si>
   <si>
     <t xml:space="preserve">care_red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enum (‘red’, ‘blue’, ‘green’, ‘yellow) FK PATIENT</t>
   </si>
   <si>
     <t xml:space="preserve">care_blue</t>
@@ -342,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -353,6 +356,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -374,8 +381,8 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,28 +439,34 @@
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>3</v>
@@ -461,44 +474,44 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,113 +519,113 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2"/>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,28 +633,28 @@
         <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>3</v>
@@ -649,30 +662,30 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,34 +693,34 @@
         <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>3</v>
@@ -715,13 +728,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>6</v>
@@ -729,73 +742,73 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>3</v>
@@ -803,84 +816,84 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tables spreadsheet and removed MEDICATION, BILL, and PAYMENT tables. Data like bill_amount, med_morn, med_noon, med_night are now in the PATIENT table
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -64,73 +64,76 @@
     <t xml:space="preserve">Varchar(255) NOT NULL</t>
   </si>
   <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date NOT NULL</t>
+  </si>
+  <si>
     <t xml:space="preserve">CARE</t>
   </si>
   <si>
-    <t xml:space="preserve">password</t>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varchar(10)</t>
   </si>
   <si>
     <t xml:space="preserve">record_id</t>
   </si>
   <si>
-    <t xml:space="preserve">dob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date NOT NULL</t>
+    <t xml:space="preserve">approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool</t>
   </si>
   <si>
     <t xml:space="preserve">med_morn</t>
   </si>
   <si>
-    <t xml:space="preserve">bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varchar(10)</t>
+    <t xml:space="preserve">role_id FK (ACCESS_ROLES)</t>
   </si>
   <si>
     <t xml:space="preserve">med_noon</t>
   </si>
   <si>
-    <t xml:space="preserve">approved</t>
-  </si>
-  <si>
     <t xml:space="preserve">med_night</t>
   </si>
   <si>
-    <t xml:space="preserve">role_id FK (ACCESS_ROLES)</t>
+    <t xml:space="preserve">PATIENT</t>
   </si>
   <si>
     <t xml:space="preserve">breakfast</t>
   </si>
   <si>
-    <t xml:space="preserve">PATIENT</t>
+    <t xml:space="preserve">patient_id</t>
   </si>
   <si>
     <t xml:space="preserve">lunch</t>
   </si>
   <si>
-    <t xml:space="preserve">patient_id</t>
+    <t xml:space="preserve">family_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varchar(20)</t>
   </si>
   <si>
     <t xml:space="preserve">dinner</t>
   </si>
   <si>
-    <t xml:space="preserve">family_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varchar(20)</t>
+    <t xml:space="preserve">em_fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varchar(50)</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">em_fname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varchar(50)</t>
+    <t xml:space="preserve">em_lname</t>
   </si>
   <si>
     <t xml:space="preserve">emp_id</t>
@@ -139,15 +142,12 @@
     <t xml:space="preserve">int FK (EMPLOYEE)</t>
   </si>
   <si>
-    <t xml:space="preserve">em_lname</t>
+    <t xml:space="preserve">em_phone</t>
   </si>
   <si>
     <t xml:space="preserve">int FK (PATIENT)</t>
   </si>
   <si>
-    <t xml:space="preserve">em_phone</t>
-  </si>
-  <si>
     <t xml:space="preserve">em_relation</t>
   </si>
   <si>
@@ -160,97 +160,52 @@
     <t xml:space="preserve">enum (‘red’, ‘blue’, ‘green’, ‘yellow)</t>
   </si>
   <si>
+    <t xml:space="preserve">APPOINTMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">int FK (USER)</t>
   </si>
   <si>
+    <t xml:space="preserve">appt_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar(50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appt_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int FK (PATIENT) NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doctor_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int FK (EMPLOYEE.emp_id) NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bill_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int DEFAULT 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
-    <t xml:space="preserve">APPOINTMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appt_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">hire_date</t>
   </si>
   <si>
-    <t xml:space="preserve">appt_date</t>
-  </si>
-  <si>
     <t xml:space="preserve">salary</t>
   </si>
   <si>
-    <t xml:space="preserve">int FK (PATIENT) NOT NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doctor_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int FK (EMPLOYEE.emp_id) NOT NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BILL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEDICATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bill_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bill_amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int NOT NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">creation_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varchar(25) NOT NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">due_date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">med_quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT FK (PATIENT)</t>
-  </si>
-  <si>
     <t xml:space="preserve">SCHEDULE</t>
   </si>
   <si>
-    <t xml:space="preserve">PAYMENT</t>
-  </si>
-  <si>
     <t xml:space="preserve">schedule_id</t>
   </si>
   <si>
-    <t xml:space="preserve">payment_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">payment_amount</t>
-  </si>
-  <si>
     <t xml:space="preserve">made_by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transaction_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int FK (BILL)</t>
   </si>
   <si>
     <t xml:space="preserve">supervisor_id</t>
@@ -381,8 +336,8 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,65 +408,53 @@
       <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>20</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,170 +462,184 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="B12" s="2"/>
+      <c r="D12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="D11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="E15" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>53</v>
@@ -690,15 +647,9 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="0" t="s">
         <v>55</v>
       </c>
     </row>
@@ -707,207 +658,132 @@
         <v>56</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>76</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D39:E39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Had to rename PATENT's 'group' to care_group (group is a keyword.) Also updated patient table to match recent changes
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -154,7 +154,7 @@
     <t xml:space="preserve">admission_date</t>
   </si>
   <si>
-    <t xml:space="preserve">group</t>
+    <t xml:space="preserve">care_group</t>
   </si>
   <si>
     <t xml:space="preserve">enum (‘red’, ‘blue’, ‘green’, ‘yellow)</t>
@@ -337,7 +337,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added all tables from the spreadsheet and modified some date names (date is a keyword)
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t xml:space="preserve">USER</t>
   </si>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Varchar(50)</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
+    <t xml:space="preserve">care_date</t>
   </si>
   <si>
     <t xml:space="preserve">em_lname</t>
@@ -193,16 +193,19 @@
     <t xml:space="preserve">EMPLOYEE</t>
   </si>
   <si>
+    <t xml:space="preserve">SCHEDULE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedule_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">hire_date</t>
   </si>
   <si>
+    <t xml:space="preserve">schedule_date</t>
+  </si>
+  <si>
     <t xml:space="preserve">salary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEDULE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schedule_id</t>
   </si>
   <si>
     <t xml:space="preserve">made_by</t>
@@ -334,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,7 +533,7 @@
         <v>36</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +661,9 @@
         <v>56</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,21 +673,39 @@
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="D28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="D29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,89 +715,59 @@
       <c r="B31" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="D31" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="2"/>
+      <c r="D35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="0" t="s">
+      <c r="D36" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D7:E7"/>
@@ -782,7 +775,6 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A35:B35"/>
     <mergeCell ref="D39:E39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>